<commit_message>
plots for v17 update
</commit_message>
<xml_diff>
--- a/results/Results paper VIGIL_v17.xlsx
+++ b/results/Results paper VIGIL_v17.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jayram/research/Topic/Machine Intelligence/VQA/COG/COG_publications/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszkornuta/Documents/GitHub/COG_publications/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2D1C07-D9D5-E14E-8A02-6E8DDC695448}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA268E-2CEB-714B-807A-0C55D41D76D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="67">
   <si>
     <t xml:space="preserve">Trained on </t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>(Fine-tuning)</t>
+  </si>
+  <si>
+    <t>(Zero-shot)</t>
   </si>
 </sst>
 </file>
@@ -2226,6 +2229,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2304,7 +2308,7 @@
                     <c:v> </c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v> </c:v>
+                    <c:v>(Zero-shot)</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>(Fine-tuning)</c:v>
@@ -2362,6 +2366,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2440,7 +2445,7 @@
                     <c:v> </c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v> </c:v>
+                    <c:v>(Zero-shot)</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>(Fine-tuning)</c:v>
@@ -2573,7 +2578,7 @@
                     <c:v> </c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v> </c:v>
+                    <c:v>(Zero-shot)</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>(Fine-tuning)</c:v>
@@ -2674,7 +2679,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.5"/>
+          <c:min val="0.55000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2692,7 +2697,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7808,13 +7813,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="K4:L4"/>
@@ -7824,6 +7822,13 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7833,8 +7838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950B3BD-F67F-7347-9596-8AB8CAAAC726}">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="M33" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AB56" sqref="AB56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10250,7 +10255,7 @@
     <row r="42" spans="1:30">
       <c r="A42" s="1"/>
       <c r="Q42" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R42" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
v17 plot update 2 - decimal fix
</commit_message>
<xml_diff>
--- a/results/Results paper VIGIL_v17.xlsx
+++ b/results/Results paper VIGIL_v17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszkornuta/Documents/GitHub/COG_publications/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA268E-2CEB-714B-807A-0C55D41D76D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406E32F5-CE7F-A449-B9F5-9E0A564B2ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
   </bookViews>
@@ -2500,6 +2500,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -7838,8 +7839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950B3BD-F67F-7347-9596-8AB8CAAAC726}">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M33" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AB56" sqref="AB56"/>
+    <sheetView tabSelected="1" topLeftCell="M26" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AE41" sqref="AE41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>